<commit_message>
analyse.py pushed for raspberry
</commit_message>
<xml_diff>
--- a/output/letter_incorrect_percentage.xlsx
+++ b/output/letter_incorrect_percentage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -998,83 +998,83 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-30 15:24:51</t>
+          <t>2024-08-30 16:01:26</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>73.91304347826086</v>
+        <v>15.38461538461539</v>
       </c>
       <c r="C7" t="n">
-        <v>87.5</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>68.75</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>65.85365853658537</v>
+        <v>7.692307692307693</v>
       </c>
       <c r="G7" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="I7" t="n">
-        <v>62.5</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>77.14285714285715</v>
+        <v>30</v>
       </c>
       <c r="K7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>76.92307692307693</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>73.07692307692307</v>
+        <v>10</v>
       </c>
       <c r="P7" t="n">
-        <v>77.77777777777779</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="Q7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>53.33333333333334</v>
+        <v>25</v>
       </c>
       <c r="T7" t="n">
-        <v>66.66666666666666</v>
+        <v>25</v>
       </c>
       <c r="U7" t="n">
-        <v>77.27272727272727</v>
+        <v>7.692307692307693</v>
       </c>
       <c r="V7" t="n">
-        <v>81.81818181818183</v>
+        <v>100</v>
       </c>
       <c r="W7" t="n">
         <v>100</v>
       </c>
       <c r="X7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1083,83 +1083,83 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-30 15:25:34</t>
+          <t>2024-08-30 16:02:53</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>73.91304347826086</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="C8" t="n">
-        <v>87.5</v>
+        <v>75</v>
       </c>
       <c r="D8" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E8" t="n">
-        <v>68.75</v>
+        <v>41.17647058823529</v>
       </c>
       <c r="F8" t="n">
-        <v>70.73170731707317</v>
+        <v>49.0566037735849</v>
       </c>
       <c r="G8" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H8" t="n">
         <v>80</v>
       </c>
       <c r="I8" t="n">
-        <v>62.5</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K8" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>75</v>
+        <v>42.85714285714285</v>
       </c>
       <c r="M8" t="n">
-        <v>76.92307692307693</v>
+        <v>47.82608695652174</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>73.07692307692307</v>
+        <v>51.61290322580645</v>
       </c>
       <c r="P8" t="n">
-        <v>76.92307692307693</v>
+        <v>54.16666666666666</v>
       </c>
       <c r="Q8" t="n">
-        <v>100</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>53.33333333333334</v>
+        <v>50</v>
       </c>
       <c r="T8" t="n">
-        <v>66.66666666666666</v>
+        <v>57.14285714285714</v>
       </c>
       <c r="U8" t="n">
-        <v>72.72727272727273</v>
+        <v>50.90909090909091</v>
       </c>
       <c r="V8" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="W8" t="n">
         <v>100</v>
       </c>
       <c r="X8" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="Y8" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>100</v>
+        <v>45.45454545454545</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
@@ -1168,35 +1168,35 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-30 15:31:21</t>
+          <t>2024-08-30 16:13:05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>48.27586206896552</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>68.42105263157895</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -1205,46 +1205,46 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>53.84615384615385</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>68.75</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>85.71428571428571</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1253,74 +1253,74 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-30 15:36:32</t>
+          <t>2024-08-30 16:18:04</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76.92307692307693</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>83.33333333333334</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>84.61538461538461</v>
+        <v>20</v>
       </c>
       <c r="G10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
+        <v>100</v>
+      </c>
+      <c r="J10" t="n">
+        <v>60</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>50</v>
       </c>
-      <c r="J10" t="n">
-        <v>70</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>100</v>
-      </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>87.5</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>81.81818181818183</v>
+        <v>100</v>
       </c>
       <c r="U10" t="n">
-        <v>61.53846153846154</v>
+        <v>100</v>
       </c>
       <c r="V10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
         <v>100</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
@@ -1338,35 +1338,35 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-30 15:45:53</t>
+          <t>2024-08-30 16:19:59</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>83.33333333333334</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F11" t="n">
-        <v>84.61538461538461</v>
+        <v>100</v>
       </c>
       <c r="G11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1375,37 +1375,37 @@
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>100</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
         <v>100</v>
       </c>
       <c r="Q11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>85.71428571428571</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>61.53846153846154</v>
+        <v>100</v>
       </c>
       <c r="V11" t="n">
         <v>100</v>
       </c>
       <c r="W11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
         <v>100</v>
@@ -1423,86 +1423,171 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-30 15:47:18</t>
+          <t>2024-08-30 16:22:16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>30.76923076923077</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>33.33333333333333</v>
       </c>
-      <c r="E12" t="n">
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>100</v>
+      </c>
+      <c r="V12" t="n">
+        <v>100</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>100</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-30 16:53:33</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
         <v>33.33333333333333</v>
       </c>
-      <c r="F12" t="n">
-        <v>23.07692307692308</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
         <v>50</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>40</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>25</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>20</v>
-      </c>
-      <c r="P12" t="n">
-        <v>55.55555555555556</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>42.85714285714285</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>62.5</v>
-      </c>
-      <c r="T12" t="n">
-        <v>54.54545454545454</v>
-      </c>
-      <c r="U12" t="n">
-        <v>15.38461538461539</v>
-      </c>
-      <c r="V12" t="n">
-        <v>100</v>
-      </c>
-      <c r="W12" t="n">
-        <v>100</v>
-      </c>
-      <c r="X12" t="n">
-        <v>66.66666666666666</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>0</v>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>50</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>100</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a command line arg file for server
</commit_message>
<xml_diff>
--- a/output/letter_incorrect_percentage.xlsx
+++ b/output/letter_incorrect_percentage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,6 +1760,91 @@
         <v>100</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-04 16:28:43</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" t="n">
+        <v>100</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>100</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>50</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="P16" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>100</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>100</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
json format data export in analyse_for_server
</commit_message>
<xml_diff>
--- a/output/letter_incorrect_percentage.xlsx
+++ b/output/letter_incorrect_percentage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA16"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1845,6 +1845,91 @@
         <v>100</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-04 16:57:08</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>50</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>50</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>100</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>